<commit_message>
Issue with timeslice in RSD
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_A_SYS_SAD_1TS.xlsx
+++ b/SuppXLS/Scen_A_SYS_SAD_1TS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EEBEBB-8212-4149-8336-90BC2DB6B9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112DAC7C-C95F-4222-935A-7DEA28B79379}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="12" r:id="rId1"/>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="91">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -612,6 +612,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -621,11 +626,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1330,9 +1330,9 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="rsdsol" displayName="rsdsol" ref="B2:I3" totalsRowShown="0">
-  <autoFilter ref="B2:I3" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="rsdsol" displayName="rsdsol" ref="B2:AI3" totalsRowShown="0">
+  <autoFilter ref="B2:AI3" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TimeSlice"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Attribute"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Year"/>
@@ -1341,30 +1341,82 @@
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Pset_CI"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="IE"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="National"/>
+    <tableColumn id="9" xr3:uid="{2CAA8B55-B165-4CF0-AE47-C80ADE888F38}" name="IE-CW"/>
+    <tableColumn id="10" xr3:uid="{EF812373-DCC0-4145-BA9C-F7A0D096E5F3}" name="IE-KK"/>
+    <tableColumn id="11" xr3:uid="{8DFAB093-2B8C-43E7-AECD-2CF3F41F49B2}" name="IE-LS"/>
+    <tableColumn id="12" xr3:uid="{89238188-0395-40C4-B347-A608A1CE291E}" name="IE-LD"/>
+    <tableColumn id="13" xr3:uid="{E19C891F-C882-4BE5-AD41-67004AA4D1DA}" name="IE-LH"/>
+    <tableColumn id="14" xr3:uid="{22F6EDAA-B1E8-4ACA-A211-B6B5BDEA16FB}" name="IE-OY"/>
+    <tableColumn id="15" xr3:uid="{8AB49BCD-35C1-4178-BC35-CC2905B026B3}" name="IE-WH"/>
+    <tableColumn id="16" xr3:uid="{D9BDB104-573B-4215-B0B3-DC1ABB74C25F}" name="IE-WX"/>
+    <tableColumn id="17" xr3:uid="{AB86FDF8-150E-4E3A-8566-96BFFDE9B439}" name="IE-CE"/>
+    <tableColumn id="18" xr3:uid="{2BC6271F-21D3-40B6-BD1D-1F1B5388BDCA}" name="IE-KY"/>
+    <tableColumn id="19" xr3:uid="{A31E1446-5388-45E6-9F5A-36982A67F5C0}" name="IE-TA"/>
+    <tableColumn id="20" xr3:uid="{6E3FC3BB-3083-485C-BA4D-866820F23945}" name="IE-LM"/>
+    <tableColumn id="21" xr3:uid="{E4CD5152-E4B2-43CB-8640-BDD51F3C81AC}" name="IE-MO"/>
+    <tableColumn id="22" xr3:uid="{D361299C-C817-4DB6-BB27-DAF543257CC5}" name="IE-RN"/>
+    <tableColumn id="23" xr3:uid="{A53766AE-91F0-4D77-AC71-1F83BC1C28C4}" name="IE-SO"/>
+    <tableColumn id="24" xr3:uid="{55BD9A4A-2BC5-439A-8253-48E364A44623}" name="IE-CN"/>
+    <tableColumn id="25" xr3:uid="{282DC8C4-649C-40C8-8A57-1CA2E394C16C}" name="IE-DL"/>
+    <tableColumn id="26" xr3:uid="{DCEBCF7B-568F-49C6-9733-27761666ADF3}" name="IE-MN"/>
+    <tableColumn id="27" xr3:uid="{554D8EB4-D3B2-4F11-B1D4-C93B609829D1}" name="IE-D"/>
+    <tableColumn id="28" xr3:uid="{30E52CCF-ABBB-474B-97BC-3C3AC3485BB0}" name="IE-KE"/>
+    <tableColumn id="29" xr3:uid="{186AA6D7-B8C6-4090-B3B2-8B3C7C950A1D}" name="IE-MH"/>
+    <tableColumn id="30" xr3:uid="{A43B205E-E364-4B3E-B3F4-882BCA623E51}" name="IE-WW"/>
+    <tableColumn id="31" xr3:uid="{C9B57BAF-CDBB-4821-B3E9-7550B0CE77FB}" name="IE-CO"/>
+    <tableColumn id="32" xr3:uid="{40D42D76-3B04-4875-9C13-966B57769DBC}" name="IE-LK"/>
+    <tableColumn id="33" xr3:uid="{7E806A56-D404-4883-B96F-A9B8D55A3BFF}" name="IE-WD"/>
+    <tableColumn id="34" xr3:uid="{7B0069A0-66A4-47AA-9531-6B10E81E22EA}" name="IE-G"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="rsd_sh" displayName="rsd_sh" ref="B2:G3" totalsRowShown="0">
-  <autoFilter ref="B2:G3" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="rsd_sh" displayName="rsd_sh" ref="B2:AG3" totalsRowShown="0">
+  <autoFilter ref="B2:AG3" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="TimeSlice"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Attribute"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Year"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Cset_CN"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="IE"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="National"/>
+    <tableColumn id="7" xr3:uid="{21B1A523-8FEA-4802-A024-3483CC1C88D3}" name="IE-CW"/>
+    <tableColumn id="8" xr3:uid="{41F84DBE-17B3-45C0-852B-AFDA9FE5C8DD}" name="IE-KK"/>
+    <tableColumn id="9" xr3:uid="{9603AC97-5A65-4070-A6A6-D55BFCE7EECA}" name="IE-LS"/>
+    <tableColumn id="10" xr3:uid="{5A3BB424-B503-4415-A366-0D0DE17AF4ED}" name="IE-LD"/>
+    <tableColumn id="11" xr3:uid="{A5C0C334-2157-4D1B-A609-4F3E88E71334}" name="IE-LH"/>
+    <tableColumn id="12" xr3:uid="{FEFB002F-7154-4FF8-A503-AAE828A58CCF}" name="IE-OY"/>
+    <tableColumn id="13" xr3:uid="{FB0A94C1-2CC0-4C82-9212-45291696710D}" name="IE-WH"/>
+    <tableColumn id="14" xr3:uid="{91DF723F-6623-48CB-8D08-5BB33E603164}" name="IE-WX"/>
+    <tableColumn id="15" xr3:uid="{728E98AE-0FD1-498A-8489-8036ED6F19C0}" name="IE-CE"/>
+    <tableColumn id="16" xr3:uid="{6F604DD4-3BC8-49EB-A8EF-E7E08370C0A1}" name="IE-KY"/>
+    <tableColumn id="17" xr3:uid="{C50A0A08-C28D-4114-8B82-15DE99E2D735}" name="IE-TA"/>
+    <tableColumn id="18" xr3:uid="{C4C7CAFC-6FDC-4788-B448-A0913C8FCE36}" name="IE-LM"/>
+    <tableColumn id="19" xr3:uid="{9EE0B161-7C3D-4A0B-91D6-912174A60646}" name="IE-MO"/>
+    <tableColumn id="20" xr3:uid="{82615C0F-102B-40B7-9697-5EA81FA52328}" name="IE-RN"/>
+    <tableColumn id="21" xr3:uid="{05F85686-E7D4-4128-8129-BAAF0EF0C9E7}" name="IE-SO"/>
+    <tableColumn id="22" xr3:uid="{6D0385CF-B756-40EF-8195-6BD06D74111F}" name="IE-CN"/>
+    <tableColumn id="23" xr3:uid="{0404144B-B9F7-4108-960F-CA8E9C698240}" name="IE-DL"/>
+    <tableColumn id="24" xr3:uid="{86F572A4-4AA7-41AE-B8D2-29AE11D761FB}" name="IE-MN"/>
+    <tableColumn id="25" xr3:uid="{2414E9F5-A0B6-4A8E-BF08-E5B27BC2B072}" name="IE-D"/>
+    <tableColumn id="26" xr3:uid="{94193197-A7F4-4580-9553-A029CE4EC724}" name="IE-KE"/>
+    <tableColumn id="27" xr3:uid="{AD51C6F5-4E34-406E-B609-287D0C8AA992}" name="IE-MH"/>
+    <tableColumn id="28" xr3:uid="{D324E7C4-65BA-4B10-94CA-B5A7D39AB34C}" name="IE-WW"/>
+    <tableColumn id="29" xr3:uid="{8B1C2E22-1A9D-404A-9E12-ECE29C56846A}" name="IE-CO"/>
+    <tableColumn id="30" xr3:uid="{45DE2179-BFE8-4780-9E0D-6B3C7C94A3BB}" name="IE-LK"/>
+    <tableColumn id="31" xr3:uid="{AC446561-7168-44D1-8E82-714DF5541264}" name="IE-WD"/>
+    <tableColumn id="32" xr3:uid="{69A3F845-C3B5-4A4B-81AE-48A85C52A28B}" name="IE-G"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="rsd_rtft" displayName="rsd_rtft" ref="B2:H3" totalsRowShown="0">
-  <autoFilter ref="B2:H3" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="rsd_rtft" displayName="rsd_rtft" ref="B2:AH3" totalsRowShown="0">
+  <autoFilter ref="B2:AH3" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+  <tableColumns count="33">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="TimeSlice"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Attribute"/>
     <tableColumn id="7" xr3:uid="{DA5FA9F4-D4B7-44E0-A803-2D2586DBF9CB}" name="LimType"/>
@@ -1372,21 +1424,73 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Pset_PN"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="IE"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="National"/>
+    <tableColumn id="8" xr3:uid="{DCA512E4-1372-4872-B8C1-7091A3CAF689}" name="IE-CW"/>
+    <tableColumn id="9" xr3:uid="{566FF8F8-E4D2-481D-B77F-B89E2C061E8F}" name="IE-KK"/>
+    <tableColumn id="10" xr3:uid="{96908983-EDDD-4B66-AB28-70FAFCD5EB1F}" name="IE-LS"/>
+    <tableColumn id="11" xr3:uid="{5CF342C5-A881-441E-AAEA-5F5946FF4525}" name="IE-LD"/>
+    <tableColumn id="12" xr3:uid="{CB36D318-3CCB-429C-B061-2B4E24BF2F69}" name="IE-LH"/>
+    <tableColumn id="13" xr3:uid="{E41A18EB-2FAD-491D-B89C-EFEA9A94D466}" name="IE-OY"/>
+    <tableColumn id="14" xr3:uid="{BFBD7E67-FF2B-48B2-999A-5C09877924DC}" name="IE-WH"/>
+    <tableColumn id="15" xr3:uid="{6E329289-D59C-4A24-BE49-725E1A2A074B}" name="IE-WX"/>
+    <tableColumn id="16" xr3:uid="{B04AF27A-5ABC-437B-A847-E58752661729}" name="IE-CE"/>
+    <tableColumn id="17" xr3:uid="{2BC04174-84AE-4C71-8515-9D011DBB7297}" name="IE-KY"/>
+    <tableColumn id="18" xr3:uid="{B7DC9DDD-A501-4AB3-8C77-90BCCB2E2188}" name="IE-TA"/>
+    <tableColumn id="19" xr3:uid="{E945BE94-B411-4C86-AB69-FFBE99F1B07E}" name="IE-LM"/>
+    <tableColumn id="20" xr3:uid="{932BEEF0-0F33-4C1B-A4A2-64E938F582D6}" name="IE-MO"/>
+    <tableColumn id="21" xr3:uid="{DCBAD216-DFBB-4A5E-A408-4442DE9A4110}" name="IE-RN"/>
+    <tableColumn id="22" xr3:uid="{D8FDE298-E73E-4117-9875-B0D91018E53C}" name="IE-SO"/>
+    <tableColumn id="23" xr3:uid="{880B3E3A-ADB5-4130-A4B1-BB074F9E2E24}" name="IE-CN"/>
+    <tableColumn id="24" xr3:uid="{1B5E46A8-6293-4452-9B07-87717E049883}" name="IE-DL"/>
+    <tableColumn id="25" xr3:uid="{B9FC05E0-476B-425B-B554-B735E4F5B623}" name="IE-MN"/>
+    <tableColumn id="26" xr3:uid="{51D06462-B467-430A-865B-36DB24AE95AE}" name="IE-D"/>
+    <tableColumn id="27" xr3:uid="{EBC5062F-9FB0-4AF2-A0D5-513B604BBF23}" name="IE-KE"/>
+    <tableColumn id="28" xr3:uid="{B2B8DA62-694E-4DDB-A50D-A3AE8279A5FC}" name="IE-MH"/>
+    <tableColumn id="29" xr3:uid="{E8F388D0-04FF-4C26-A274-D97157682180}" name="IE-WW"/>
+    <tableColumn id="30" xr3:uid="{6563318E-6F11-4283-AF55-FF77AC91DAF5}" name="IE-CO"/>
+    <tableColumn id="31" xr3:uid="{671C6FB4-D917-455A-919A-EF6ABAE25918}" name="IE-LK"/>
+    <tableColumn id="32" xr3:uid="{38E1DE3C-DF1B-4B6C-A692-2AD4DF569440}" name="IE-WD"/>
+    <tableColumn id="33" xr3:uid="{CFCD75F4-4676-495E-8FF2-180B509651FA}" name="IE-G"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="rsd_oe_dem" displayName="rsd_oe_dem" ref="B2:G3" totalsRowShown="0">
-  <autoFilter ref="B2:G3" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="rsd_oe_dem" displayName="rsd_oe_dem" ref="B2:AG3" totalsRowShown="0">
+  <autoFilter ref="B2:AG3" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+  <tableColumns count="32">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TimeSlice"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Attribute"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Year"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Cset_CN"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="IE"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="National"/>
+    <tableColumn id="7" xr3:uid="{EC610DF9-E4E7-41C1-9F3B-5AA74912475E}" name="IE-CW"/>
+    <tableColumn id="8" xr3:uid="{A36075A4-5E97-494C-8F92-AE1146B781CA}" name="IE-KK"/>
+    <tableColumn id="9" xr3:uid="{8D4F5321-92C0-4E60-AA66-E1E12110C8EE}" name="IE-LS"/>
+    <tableColumn id="10" xr3:uid="{620FEDD9-8C99-466C-A10F-5E3F2C0B98C8}" name="IE-LD"/>
+    <tableColumn id="11" xr3:uid="{23102628-F969-4CB0-BA20-5B620DC3D641}" name="IE-LH"/>
+    <tableColumn id="12" xr3:uid="{596F087A-7C2F-4ACB-AB9D-9E7D1D23A198}" name="IE-OY"/>
+    <tableColumn id="13" xr3:uid="{BA34CB73-7B43-4E61-843C-C21370CC3E8B}" name="IE-WH"/>
+    <tableColumn id="14" xr3:uid="{EC261330-DC73-40F2-ADAE-20124BE1ED55}" name="IE-WX"/>
+    <tableColumn id="15" xr3:uid="{C65D2C5B-F433-468B-992C-15F652190CC2}" name="IE-CE"/>
+    <tableColumn id="16" xr3:uid="{76D798AA-C0CD-4222-A4F6-F6D83E69C47E}" name="IE-KY"/>
+    <tableColumn id="17" xr3:uid="{87EB76A7-760A-4070-BCED-1EB70BE2E626}" name="IE-TA"/>
+    <tableColumn id="18" xr3:uid="{5A65D867-E694-43EC-B76C-D341B9584E44}" name="IE-LM"/>
+    <tableColumn id="19" xr3:uid="{6563DEDD-B3F6-402D-921C-0F15FD79C70D}" name="IE-MO"/>
+    <tableColumn id="20" xr3:uid="{314C09F3-0010-494A-A4D2-93E7EB3B70E8}" name="IE-RN"/>
+    <tableColumn id="21" xr3:uid="{1F90FC44-78D7-4228-8F72-C0F5D81521B9}" name="IE-SO"/>
+    <tableColumn id="22" xr3:uid="{C3803B25-E5E2-4865-9DCC-4DF459484439}" name="IE-CN"/>
+    <tableColumn id="23" xr3:uid="{C7D3F892-ADC0-408C-9A69-E863F986B9E3}" name="IE-DL"/>
+    <tableColumn id="24" xr3:uid="{46B820EB-34CE-44E5-BB07-A545AD903792}" name="IE-MN"/>
+    <tableColumn id="25" xr3:uid="{9441BE26-B8EC-4D1E-BFCC-B8FA43E7D030}" name="IE-D"/>
+    <tableColumn id="26" xr3:uid="{A4625807-1209-455A-AD47-8D03D226A2DA}" name="IE-KE"/>
+    <tableColumn id="27" xr3:uid="{94AD9825-2A45-4B32-BDF9-9EE9ABD2F651}" name="IE-MH"/>
+    <tableColumn id="28" xr3:uid="{19F6DC98-EEDE-436A-BD24-ED32C1B0AA05}" name="IE-WW"/>
+    <tableColumn id="29" xr3:uid="{4B570DA7-B1C5-46CD-8C4C-3B72EF728923}" name="IE-CO"/>
+    <tableColumn id="30" xr3:uid="{D93CB9C6-F682-46DB-A6F9-585E0F1F6E08}" name="IE-LK"/>
+    <tableColumn id="31" xr3:uid="{FD70ABE1-6353-4AE4-AE56-2CD05082E75E}" name="IE-WD"/>
+    <tableColumn id="32" xr3:uid="{F514900A-774C-476B-B59D-06B59BA52225}" name="IE-G"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2128,12 +2232,12 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="5"/>
@@ -2217,11 +2321,11 @@
       <c r="A19" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="11"/>
@@ -2249,11 +2353,11 @@
       <c r="A20" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="11"/>
@@ -2341,11 +2445,11 @@
       <c r="A23" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -2371,9 +2475,9 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -2429,11 +2533,11 @@
       <c r="A26" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -2549,11 +2653,11 @@
       <c r="A30" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="2"/>
@@ -2581,11 +2685,11 @@
       <c r="A31" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="2"/>
@@ -4858,27 +4962,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E87912A-05C7-48D9-8B04-811783F0B11F}">
   <dimension ref="B3:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="19" t="s">
         <v>85</v>
       </c>
       <c r="L4" t="s">
@@ -4901,13 +5005,13 @@
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="20" t="s">
         <v>89</v>
       </c>
       <c r="L5">
@@ -4930,9 +5034,9 @@
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
       <c r="L6">
         <v>1</v>
       </c>
@@ -4953,9 +5057,9 @@
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
       <c r="L7">
         <v>2</v>
       </c>
@@ -4976,9 +5080,9 @@
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
       <c r="L8">
         <v>3</v>
       </c>
@@ -5039,7 +5143,7 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="24"/>
+      <c r="B11" s="21"/>
       <c r="L11">
         <v>6</v>
       </c>
@@ -5060,7 +5164,7 @@
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="24"/>
+      <c r="B12" s="21"/>
       <c r="L12">
         <v>7</v>
       </c>
@@ -5075,7 +5179,7 @@
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="24"/>
+      <c r="B13" s="21"/>
       <c r="L13">
         <v>8</v>
       </c>
@@ -5090,7 +5194,7 @@
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="24"/>
+      <c r="B14" s="21"/>
       <c r="L14">
         <v>9</v>
       </c>
@@ -5105,7 +5209,7 @@
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="24"/>
+      <c r="B15" s="21"/>
       <c r="L15">
         <v>10</v>
       </c>
@@ -5120,7 +5224,7 @@
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="24"/>
+      <c r="B16" s="21"/>
       <c r="L16">
         <v>11</v>
       </c>
@@ -5135,7 +5239,7 @@
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="24"/>
+      <c r="B17" s="21"/>
       <c r="R17">
         <v>12</v>
       </c>
@@ -5454,20 +5558,20 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:I3"/>
+  <dimension ref="B1:AI3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AI7" sqref="AI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -5492,8 +5596,86 @@
       <c r="I2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V2" t="s">
+        <v>25</v>
+      </c>
+      <c r="W2" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>31</v>
       </c>
@@ -5516,6 +5698,84 @@
         <v>0.10802</v>
       </c>
       <c r="I3">
+        <v>0.10802</v>
+      </c>
+      <c r="J3">
+        <v>0.10802</v>
+      </c>
+      <c r="K3">
+        <v>0.10802</v>
+      </c>
+      <c r="L3">
+        <v>0.10802</v>
+      </c>
+      <c r="M3">
+        <v>0.10802</v>
+      </c>
+      <c r="N3">
+        <v>0.10802</v>
+      </c>
+      <c r="O3">
+        <v>0.10802</v>
+      </c>
+      <c r="P3">
+        <v>0.10802</v>
+      </c>
+      <c r="Q3">
+        <v>0.10802</v>
+      </c>
+      <c r="R3">
+        <v>0.10802</v>
+      </c>
+      <c r="S3">
+        <v>0.10802</v>
+      </c>
+      <c r="T3">
+        <v>0.10802</v>
+      </c>
+      <c r="U3">
+        <v>0.10802</v>
+      </c>
+      <c r="V3">
+        <v>0.10802</v>
+      </c>
+      <c r="W3">
+        <v>0.10802</v>
+      </c>
+      <c r="X3">
+        <v>0.10802</v>
+      </c>
+      <c r="Y3">
+        <v>0.10802</v>
+      </c>
+      <c r="Z3">
+        <v>0.10802</v>
+      </c>
+      <c r="AA3">
+        <v>0.10802</v>
+      </c>
+      <c r="AB3">
+        <v>0.10802</v>
+      </c>
+      <c r="AC3">
+        <v>0.10802</v>
+      </c>
+      <c r="AD3">
+        <v>0.10802</v>
+      </c>
+      <c r="AE3">
+        <v>0.10802</v>
+      </c>
+      <c r="AF3">
+        <v>0.10802</v>
+      </c>
+      <c r="AG3">
+        <v>0.10802</v>
+      </c>
+      <c r="AH3">
+        <v>0.10802</v>
+      </c>
+      <c r="AI3">
         <v>0.10802</v>
       </c>
     </row>
@@ -5531,18 +5791,20 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B1:G3"/>
+  <dimension ref="B1:AG3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AG2" sqref="H2:AG2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -5561,8 +5823,86 @@
       <c r="G2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>31</v>
       </c>
@@ -5579,6 +5919,84 @@
         <v>1</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
         <v>1</v>
       </c>
     </row>
@@ -5594,20 +6012,20 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="B1:H3"/>
+  <dimension ref="B1:AH3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AH2" sqref="I2:AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -5629,8 +6047,86 @@
       <c r="H2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U2" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" t="s">
+        <v>27</v>
+      </c>
+      <c r="X2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>31</v>
       </c>
@@ -5650,6 +6146,84 @@
         <v>1</v>
       </c>
       <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
+        <v>1</v>
+      </c>
+      <c r="AH3">
         <v>1</v>
       </c>
     </row>
@@ -5665,18 +6239,20 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="B1:G3"/>
+  <dimension ref="B1:AG3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AF5" sqref="AF5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -5695,8 +6271,86 @@
       <c r="G2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>31</v>
       </c>
@@ -5713,6 +6367,84 @@
         <v>1</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>1</v>
+      </c>
+      <c r="AF3">
+        <v>1</v>
+      </c>
+      <c r="AG3">
         <v>1</v>
       </c>
     </row>
@@ -5873,7 +6605,9 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="B1:AG3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:AG2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>